<commit_message>
feat: implement new tmeplate
</commit_message>
<xml_diff>
--- a/S5251/Input from proponent/Proponent PQ curve.xlsx
+++ b/S5251/Input from proponent/Proponent PQ curve.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Energy Startup\Code repository\S5251\Input from proponent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Energy Startup\Code repository\S5251\Input from proponent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1F2350-6E03-45C5-B9F6-80D73313A437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED850EE-165A-4F78-83F4-5ED1E78D92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>P</t>
   </si>
   <si>
     <t>Q</t>
-  </si>
-  <si>
-    <t>Voltage V</t>
   </si>
 </sst>
 </file>
@@ -1386,276 +1383,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>950000</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>950000</v>
       </c>
       <c r="B3">
         <v>360000</v>
       </c>
-      <c r="C3">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>850000</v>
       </c>
       <c r="B4">
         <v>324000</v>
       </c>
-      <c r="C4">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>750000</v>
       </c>
       <c r="B5">
         <v>291600</v>
       </c>
-      <c r="C5">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>650000</v>
       </c>
       <c r="B6">
         <v>262440</v>
       </c>
-      <c r="C6">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>550000</v>
       </c>
       <c r="B7">
         <v>250000</v>
       </c>
-      <c r="C7">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>450000</v>
       </c>
       <c r="B8">
         <v>200000</v>
       </c>
-      <c r="C8">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>350000</v>
       </c>
       <c r="B9">
         <v>200000</v>
       </c>
-      <c r="C9">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>250000</v>
       </c>
       <c r="B10">
         <v>200000</v>
       </c>
-      <c r="C10">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>150000</v>
       </c>
       <c r="B11">
         <v>200000</v>
       </c>
-      <c r="C11">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>50000</v>
       </c>
       <c r="B12">
         <v>200000</v>
       </c>
-      <c r="C12">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="B13">
         <v>200000</v>
       </c>
-      <c r="C13">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
       <c r="B14">
         <v>-200000</v>
       </c>
-      <c r="C14">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>150000</v>
       </c>
       <c r="B15">
         <v>-200000</v>
       </c>
-      <c r="C15">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>250000</v>
       </c>
       <c r="B16">
         <v>-200000</v>
       </c>
-      <c r="C16">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>350000</v>
       </c>
       <c r="B17">
         <v>-200000</v>
       </c>
-      <c r="C17">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>450000</v>
       </c>
       <c r="B18">
         <v>-200000</v>
       </c>
-      <c r="C18">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>550000</v>
       </c>
       <c r="B19">
         <v>-250000</v>
       </c>
-      <c r="C19">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>650000</v>
       </c>
       <c r="B20">
         <v>-275000</v>
       </c>
-      <c r="C20">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>750000</v>
       </c>
       <c r="B21">
         <v>-277500</v>
       </c>
-      <c r="C21">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>850000</v>
       </c>
       <c r="B22">
         <v>-277750</v>
       </c>
-      <c r="C22">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>950000</v>
       </c>
       <c r="B23">
         <v>-277775</v>
       </c>
-      <c r="C23">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>950000</v>
       </c>
       <c r="B24">
         <v>0</v>
-      </c>
-      <c r="C24">
-        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>